<commit_message>
snowflake PDF files added in SQL folder
</commit_message>
<xml_diff>
--- a/SIM Card Details/Airtel/All Airtel Numbers/All Airtel Numbers.xlsx
+++ b/SIM Card Details/Airtel/All Airtel Numbers/All Airtel Numbers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9795" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9795" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="All SIMS" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'All SIMS'!$B$1:$L$419</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'All SIMS'!$A$1:$L$419</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Info!$A$1:$K$67</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9661" uniqueCount="1279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9731" uniqueCount="1309">
   <si>
     <t>MOBILE_NUMBER</t>
   </si>
@@ -3864,6 +3864,96 @@
   </si>
   <si>
     <t>Airtel</t>
+  </si>
+  <si>
+    <t>5754000558762</t>
+  </si>
+  <si>
+    <t>8991000905770767822</t>
+  </si>
+  <si>
+    <t>404490624645598</t>
+  </si>
+  <si>
+    <t>5754000558758</t>
+  </si>
+  <si>
+    <t>8991000905770767780</t>
+  </si>
+  <si>
+    <t>404490624647458</t>
+  </si>
+  <si>
+    <t>5754000558756</t>
+  </si>
+  <si>
+    <t>8991000905770767764</t>
+  </si>
+  <si>
+    <t>404490624647457</t>
+  </si>
+  <si>
+    <t>5754000558764</t>
+  </si>
+  <si>
+    <t>8991000905770767848</t>
+  </si>
+  <si>
+    <t>404490624645614</t>
+  </si>
+  <si>
+    <t>5754000558759</t>
+  </si>
+  <si>
+    <t>8991000905770767798</t>
+  </si>
+  <si>
+    <t>404490624645627</t>
+  </si>
+  <si>
+    <t>5754000558760</t>
+  </si>
+  <si>
+    <t>8991000905770767806</t>
+  </si>
+  <si>
+    <t>404490624645603</t>
+  </si>
+  <si>
+    <t>5754000558757</t>
+  </si>
+  <si>
+    <t>8991000905770767772</t>
+  </si>
+  <si>
+    <t>404490624645631</t>
+  </si>
+  <si>
+    <t>5754000558763</t>
+  </si>
+  <si>
+    <t>8991000905770767830</t>
+  </si>
+  <si>
+    <t>404490624645606</t>
+  </si>
+  <si>
+    <t>5754000558761</t>
+  </si>
+  <si>
+    <t>8991000905770767814</t>
+  </si>
+  <si>
+    <t>404490624647460</t>
+  </si>
+  <si>
+    <t>5754000558755</t>
+  </si>
+  <si>
+    <t>8991000905770767756</t>
+  </si>
+  <si>
+    <t>404490624645618</t>
   </si>
 </sst>
 </file>
@@ -19092,10 +19182,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:L419"/>
+  <dimension ref="A1:L429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A280" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F392" sqref="F392:F429"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34023,7 +34113,7 @@
         <v>14</v>
       </c>
       <c r="F393" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G393" s="5" t="s">
         <v>16</v>
@@ -34061,7 +34151,7 @@
         <v>14</v>
       </c>
       <c r="F394" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G394" s="5" t="s">
         <v>16</v>
@@ -34099,7 +34189,7 @@
         <v>14</v>
       </c>
       <c r="F395" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G395" s="5" t="s">
         <v>16</v>
@@ -34137,7 +34227,7 @@
         <v>14</v>
       </c>
       <c r="F396" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G396" s="5" t="s">
         <v>16</v>
@@ -34175,7 +34265,7 @@
         <v>14</v>
       </c>
       <c r="F397" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G397" s="5" t="s">
         <v>16</v>
@@ -34213,7 +34303,7 @@
         <v>14</v>
       </c>
       <c r="F398" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G398" s="5" t="s">
         <v>16</v>
@@ -34251,7 +34341,7 @@
         <v>14</v>
       </c>
       <c r="F399" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G399" s="5" t="s">
         <v>16</v>
@@ -34289,7 +34379,7 @@
         <v>14</v>
       </c>
       <c r="F400" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G400" s="5" t="s">
         <v>16</v>
@@ -34327,7 +34417,7 @@
         <v>14</v>
       </c>
       <c r="F401" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G401" s="5" t="s">
         <v>16</v>
@@ -34365,7 +34455,7 @@
         <v>14</v>
       </c>
       <c r="F402" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G402" s="5" t="s">
         <v>16</v>
@@ -34403,7 +34493,7 @@
         <v>14</v>
       </c>
       <c r="F403" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G403" s="5" t="s">
         <v>16</v>
@@ -34441,7 +34531,7 @@
         <v>14</v>
       </c>
       <c r="F404" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G404" s="5" t="s">
         <v>16</v>
@@ -34479,7 +34569,7 @@
         <v>14</v>
       </c>
       <c r="F405" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G405" s="5" t="s">
         <v>16</v>
@@ -34517,7 +34607,7 @@
         <v>14</v>
       </c>
       <c r="F406" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G406" s="5" t="s">
         <v>16</v>
@@ -34555,7 +34645,7 @@
         <v>14</v>
       </c>
       <c r="F407" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G407" s="5" t="s">
         <v>16</v>
@@ -34593,7 +34683,7 @@
         <v>14</v>
       </c>
       <c r="F408" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G408" s="5" t="s">
         <v>16</v>
@@ -34631,7 +34721,7 @@
         <v>14</v>
       </c>
       <c r="F409" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G409" s="5" t="s">
         <v>16</v>
@@ -34669,7 +34759,7 @@
         <v>14</v>
       </c>
       <c r="F410" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G410" s="5" t="s">
         <v>16</v>
@@ -34707,7 +34797,7 @@
         <v>14</v>
       </c>
       <c r="F411" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G411" s="5" t="s">
         <v>16</v>
@@ -34745,7 +34835,7 @@
         <v>14</v>
       </c>
       <c r="F412" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G412" s="5" t="s">
         <v>16</v>
@@ -34783,7 +34873,7 @@
         <v>14</v>
       </c>
       <c r="F413" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G413" s="5" t="s">
         <v>16</v>
@@ -34821,7 +34911,7 @@
         <v>14</v>
       </c>
       <c r="F414" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G414" s="5" t="s">
         <v>16</v>
@@ -34859,7 +34949,7 @@
         <v>14</v>
       </c>
       <c r="F415" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G415" s="5" t="s">
         <v>16</v>
@@ -34897,7 +34987,7 @@
         <v>14</v>
       </c>
       <c r="F416" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G416" s="5" t="s">
         <v>16</v>
@@ -34935,7 +35025,7 @@
         <v>14</v>
       </c>
       <c r="F417" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G417" s="5" t="s">
         <v>16</v>
@@ -34973,7 +35063,7 @@
         <v>14</v>
       </c>
       <c r="F418" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G418" s="5" t="s">
         <v>16</v>
@@ -35011,7 +35101,7 @@
         <v>14</v>
       </c>
       <c r="F419" s="5" t="s">
-        <v>745</v>
+        <v>15</v>
       </c>
       <c r="G419" s="5" t="s">
         <v>16</v>
@@ -35032,8 +35122,287 @@
         <v>18</v>
       </c>
     </row>
+    <row r="420" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A420" s="3" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B420" s="5" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C420" s="5" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D420" s="5" t="s">
+        <v>1281</v>
+      </c>
+      <c r="E420" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F420" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G420" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H420" s="5"/>
+      <c r="I420" s="5"/>
+      <c r="J420" s="5"/>
+      <c r="K420" s="5"/>
+      <c r="L420" s="5"/>
+    </row>
+    <row r="421" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A421" s="3" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B421" s="5" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C421" s="5" t="s">
+        <v>1283</v>
+      </c>
+      <c r="D421" s="5" t="s">
+        <v>1284</v>
+      </c>
+      <c r="E421" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F421" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G421" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H421" s="5"/>
+      <c r="I421" s="5"/>
+      <c r="J421" s="5"/>
+      <c r="K421" s="5"/>
+      <c r="L421" s="5"/>
+    </row>
+    <row r="422" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A422" s="3" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B422" s="5" t="s">
+        <v>1285</v>
+      </c>
+      <c r="C422" s="5" t="s">
+        <v>1286</v>
+      </c>
+      <c r="D422" s="5" t="s">
+        <v>1287</v>
+      </c>
+      <c r="E422" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F422" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G422" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H422" s="5"/>
+      <c r="I422" s="5"/>
+      <c r="J422" s="5"/>
+      <c r="K422" s="5"/>
+      <c r="L422" s="5"/>
+    </row>
+    <row r="423" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A423" s="3" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B423" s="5" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C423" s="5" t="s">
+        <v>1289</v>
+      </c>
+      <c r="D423" s="5" t="s">
+        <v>1290</v>
+      </c>
+      <c r="E423" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F423" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G423" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H423" s="5"/>
+      <c r="I423" s="5"/>
+      <c r="J423" s="5"/>
+      <c r="K423" s="5"/>
+      <c r="L423" s="5"/>
+    </row>
+    <row r="424" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A424" s="3" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B424" s="5" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C424" s="5" t="s">
+        <v>1292</v>
+      </c>
+      <c r="D424" s="5" t="s">
+        <v>1293</v>
+      </c>
+      <c r="E424" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F424" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G424" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H424" s="5"/>
+      <c r="I424" s="5"/>
+      <c r="J424" s="5"/>
+      <c r="K424" s="5"/>
+      <c r="L424" s="5"/>
+    </row>
+    <row r="425" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A425" s="3" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B425" s="5" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C425" s="5" t="s">
+        <v>1295</v>
+      </c>
+      <c r="D425" s="5" t="s">
+        <v>1296</v>
+      </c>
+      <c r="E425" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F425" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G425" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H425" s="5"/>
+      <c r="I425" s="5"/>
+      <c r="J425" s="5"/>
+      <c r="K425" s="5"/>
+      <c r="L425" s="5"/>
+    </row>
+    <row r="426" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A426" s="3" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B426" s="5" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C426" s="5" t="s">
+        <v>1298</v>
+      </c>
+      <c r="D426" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="E426" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F426" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G426" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H426" s="5"/>
+      <c r="I426" s="5"/>
+      <c r="J426" s="5"/>
+      <c r="K426" s="5"/>
+      <c r="L426" s="5"/>
+    </row>
+    <row r="427" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A427" s="3" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B427" s="5" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C427" s="5" t="s">
+        <v>1301</v>
+      </c>
+      <c r="D427" s="5" t="s">
+        <v>1302</v>
+      </c>
+      <c r="E427" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F427" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G427" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H427" s="5"/>
+      <c r="I427" s="5"/>
+      <c r="J427" s="5"/>
+      <c r="K427" s="5"/>
+      <c r="L427" s="5"/>
+    </row>
+    <row r="428" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A428" s="3" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B428" s="5" t="s">
+        <v>1303</v>
+      </c>
+      <c r="C428" s="5" t="s">
+        <v>1304</v>
+      </c>
+      <c r="D428" s="5" t="s">
+        <v>1305</v>
+      </c>
+      <c r="E428" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F428" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G428" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H428" s="5"/>
+      <c r="I428" s="5"/>
+      <c r="J428" s="5"/>
+      <c r="K428" s="5"/>
+      <c r="L428" s="5"/>
+    </row>
+    <row r="429" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A429" s="3" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B429" s="5" t="s">
+        <v>1306</v>
+      </c>
+      <c r="C429" s="5" t="s">
+        <v>1307</v>
+      </c>
+      <c r="D429" s="5" t="s">
+        <v>1308</v>
+      </c>
+      <c r="E429" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F429" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G429" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H429" s="5"/>
+      <c r="I429" s="5"/>
+      <c r="J429" s="5"/>
+      <c r="K429" s="5"/>
+      <c r="L429" s="5"/>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:L419"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>